<commit_message>
Update some files Add queryDB script
</commit_message>
<xml_diff>
--- a/CSV/PeriodClosingEfficiency.xlsx
+++ b/CSV/PeriodClosingEfficiency.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colig\OneDrive\Desktop\Università\Tesi_Magistrale\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DC7B01-4FA3-43B3-A374-6A178149F003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D6F165-7971-4BCE-9B90-4A3CDF859D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{768AA3F2-DC0A-4D8C-A9D1-AA78C7643DF0}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="248">
   <si>
     <t>Activity</t>
   </si>
@@ -666,15 +666,6 @@
     <t>2381 per clienti, 11382 per fornitori</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>0 = ACT32</t>
-  </si>
-  <si>
-    <t>13=ACT15</t>
-  </si>
-  <si>
     <t>TransferOpeningClosing</t>
   </si>
   <si>
@@ -799,9 +790,6 @@
   </si>
   <si>
     <t>JournalCategory Label</t>
-  </si>
-  <si>
-    <t>1,2,3,8,10 = ACT01</t>
   </si>
   <si>
     <t>ExchRateGain</t>
@@ -985,9 +973,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1025,7 +1013,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1131,7 +1119,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1273,7 +1261,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2307,8 +2295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E8F3E7-6632-4966-8F22-C2D3C3494B11}">
   <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2327,13 +2315,13 @@
         <v>179</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>180</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>181</v>
@@ -2370,7 +2358,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2387,7 +2375,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2404,7 +2392,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2421,7 +2409,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2438,7 +2426,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2455,7 +2443,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2472,7 +2460,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2489,7 +2477,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2506,7 +2494,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2523,7 +2511,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2540,7 +2528,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -2557,7 +2545,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -2574,7 +2562,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -2591,7 +2579,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -2608,7 +2596,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -2625,7 +2613,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -2642,7 +2630,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -2659,7 +2647,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -2676,7 +2664,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -2693,7 +2681,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -2710,7 +2698,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -3198,17 +3186,11 @@
         <v>183</v>
       </c>
       <c r="E51" t="s">
-        <v>202</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>204</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -3232,7 +3214,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C53">
         <v>19</v>
@@ -3249,7 +3231,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C54">
         <v>20</v>
@@ -3266,7 +3248,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C55">
         <v>20</v>
@@ -3283,7 +3265,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C56">
         <v>20</v>
@@ -3300,7 +3282,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C57">
         <v>20</v>
@@ -3317,7 +3299,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C58">
         <v>20</v>
@@ -3334,13 +3316,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C59">
         <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E59" t="s">
         <v>69</v>
@@ -3351,7 +3333,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C60">
         <v>23</v>
@@ -3368,7 +3350,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C61">
         <v>23</v>
@@ -3385,7 +3367,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C62">
         <v>23</v>
@@ -3402,7 +3384,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C63">
         <v>31</v>
@@ -3419,7 +3401,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C64">
         <v>31</v>
@@ -3436,7 +3418,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C65">
         <v>31</v>
@@ -3453,7 +3435,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C66">
         <v>31</v>
@@ -3470,7 +3452,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C67">
         <v>31</v>
@@ -3487,7 +3469,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C68">
         <v>31</v>
@@ -3504,7 +3486,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C69">
         <v>31</v>
@@ -3521,7 +3503,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C70">
         <v>31</v>
@@ -3538,7 +3520,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C71">
         <v>32</v>
@@ -3555,7 +3537,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C72">
         <v>32</v>
@@ -3572,7 +3554,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C73">
         <v>34</v>
@@ -3589,7 +3571,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C74">
         <v>34</v>
@@ -3606,7 +3588,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C75">
         <v>37</v>
@@ -3623,7 +3605,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C76">
         <v>40</v>
@@ -3640,7 +3622,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C77">
         <v>40</v>
@@ -3657,7 +3639,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C78">
         <v>41</v>
@@ -3674,7 +3656,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C79">
         <v>41</v>
@@ -3691,7 +3673,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C80">
         <v>41</v>
@@ -3708,7 +3690,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C81">
         <v>41</v>
@@ -3725,7 +3707,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C82">
         <v>41</v>
@@ -3742,7 +3724,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C83">
         <v>41</v>
@@ -3759,7 +3741,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C84">
         <v>41</v>
@@ -3776,7 +3758,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C85">
         <v>41</v>
@@ -3793,7 +3775,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C86">
         <v>42</v>
@@ -3810,7 +3792,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C87">
         <v>45</v>
@@ -3827,7 +3809,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C88">
         <v>45</v>
@@ -3844,7 +3826,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C89">
         <v>47</v>
@@ -3861,7 +3843,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C90">
         <v>48</v>
@@ -3878,7 +3860,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C91">
         <v>48</v>
@@ -3895,7 +3877,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C92">
         <v>49</v>
@@ -3912,7 +3894,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C93">
         <v>49</v>
@@ -3929,7 +3911,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C94">
         <v>51</v>
@@ -3946,7 +3928,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C95">
         <v>58</v>
@@ -3963,7 +3945,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C96">
         <v>58</v>
@@ -3980,7 +3962,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C97">
         <v>64</v>
@@ -3997,7 +3979,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C98">
         <v>65</v>
@@ -4014,7 +3996,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C99">
         <v>71</v>
@@ -4031,7 +4013,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C100">
         <v>72</v>
@@ -4048,7 +4030,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C101">
         <v>75</v>
@@ -4065,7 +4047,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C102">
         <v>76</v>
@@ -4082,7 +4064,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C103">
         <v>78</v>
@@ -4099,7 +4081,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C104">
         <v>78</v>
@@ -4116,7 +4098,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C105">
         <v>83</v>
@@ -4133,7 +4115,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C106">
         <v>121</v>
@@ -4150,7 +4132,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C107">
         <v>121</v>
@@ -4167,7 +4149,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C108">
         <v>121</v>
@@ -4184,7 +4166,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C109">
         <v>121</v>
@@ -4201,7 +4183,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C110">
         <v>122</v>
@@ -4218,7 +4200,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C111">
         <v>128</v>
@@ -4235,7 +4217,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C112">
         <v>129</v>
@@ -4252,7 +4234,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C113">
         <v>138</v>
@@ -4269,7 +4251,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C114">
         <v>144</v>
@@ -4286,7 +4268,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C115">
         <v>156</v>
@@ -4303,7 +4285,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C116">
         <v>161</v>
@@ -4320,7 +4302,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C117">
         <v>161</v>
@@ -4337,7 +4319,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C118">
         <v>161</v>
@@ -4354,7 +4336,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C119">
         <v>161</v>
@@ -4371,7 +4353,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C120">
         <v>161</v>
@@ -4388,7 +4370,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C121">
         <v>161</v>
@@ -4405,7 +4387,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C122">
         <v>162</v>
@@ -4422,7 +4404,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C123">
         <v>162</v>
@@ -4439,7 +4421,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C124">
         <v>162</v>
@@ -4456,7 +4438,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C125">
         <v>162</v>
@@ -4473,7 +4455,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C126">
         <v>162</v>
@@ -4490,7 +4472,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C127">
         <v>203</v>
@@ -4507,7 +4489,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C128">
         <v>204</v>
@@ -4524,7 +4506,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C129">
         <v>206</v>
@@ -4541,7 +4523,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C130">
         <v>212</v>
@@ -4558,7 +4540,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C131">
         <v>212</v>
@@ -4575,7 +4557,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C132">
         <v>214</v>
@@ -4592,7 +4574,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C133">
         <v>236</v>
@@ -4609,7 +4591,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C134">
         <v>236</v>
@@ -4626,13 +4608,13 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C135">
         <v>249</v>
       </c>
       <c r="D135" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E135" t="s">
         <v>69</v>

</xml_diff>